<commit_message>
modified:   completed_games_with_predictions.xlsx modified:   nba_forecast.ipynb
added: win probability percentage in the projected winners column
</commit_message>
<xml_diff>
--- a/completed_games_with_predictions.xlsx
+++ b/completed_games_with_predictions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Away team_Boston Celtics</t>
   </si>
@@ -290,9 +290,6 @@
   </si>
   <si>
     <t>Predicted_HomeWin</t>
-  </si>
-  <si>
-    <t>Predicted_HomePts</t>
   </si>
 </sst>
 </file>
@@ -650,13 +647,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CO227"/>
+  <dimension ref="A1:CN227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:93">
+    <row r="1" spans="1:92">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -933,11 +930,8 @@
       <c r="CN1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="1" t="s">
-        <v>92</v>
-      </c>
     </row>
-    <row r="2" spans="1:93">
+    <row r="2" spans="1:92">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1212,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:93">
+    <row r="3" spans="1:92">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1487,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:93">
+    <row r="4" spans="1:92">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1762,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:93">
+    <row r="5" spans="1:92">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2037,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:93">
+    <row r="6" spans="1:92">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2312,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:93">
+    <row r="7" spans="1:92">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2587,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:93">
+    <row r="8" spans="1:92">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2862,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:93">
+    <row r="9" spans="1:92">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3139,11 +3133,8 @@
       <c r="CN9">
         <v>1</v>
       </c>
-      <c r="CO9">
-        <v>123.0546875</v>
-      </c>
     </row>
-    <row r="10" spans="1:93">
+    <row r="10" spans="1:92">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3418,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:93">
+    <row r="11" spans="1:92">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3693,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:93">
+    <row r="12" spans="1:92">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3968,7 +3959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:93">
+    <row r="13" spans="1:92">
       <c r="A13">
         <v>0</v>
       </c>
@@ -4245,11 +4236,8 @@
       <c r="CN13">
         <v>0</v>
       </c>
-      <c r="CO13">
-        <v>103.171875</v>
-      </c>
     </row>
-    <row r="14" spans="1:93">
+    <row r="14" spans="1:92">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4526,11 +4514,8 @@
       <c r="CN14">
         <v>0</v>
       </c>
-      <c r="CO14">
-        <v>111.9453125</v>
-      </c>
     </row>
-    <row r="15" spans="1:93">
+    <row r="15" spans="1:92">
       <c r="A15">
         <v>0</v>
       </c>
@@ -4807,11 +4792,8 @@
       <c r="CN15">
         <v>0</v>
       </c>
-      <c r="CO15">
-        <v>106.8515625</v>
-      </c>
     </row>
-    <row r="16" spans="1:93">
+    <row r="16" spans="1:92">
       <c r="A16">
         <v>0</v>
       </c>
@@ -5086,7 +5068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:93">
+    <row r="17" spans="1:92">
       <c r="A17">
         <v>0</v>
       </c>
@@ -5363,11 +5345,8 @@
       <c r="CN17">
         <v>0</v>
       </c>
-      <c r="CO17">
-        <v>110.4296875</v>
-      </c>
     </row>
-    <row r="18" spans="1:93">
+    <row r="18" spans="1:92">
       <c r="A18">
         <v>0</v>
       </c>
@@ -5644,11 +5623,8 @@
       <c r="CN18">
         <v>1</v>
       </c>
-      <c r="CO18">
-        <v>136.7421875</v>
-      </c>
     </row>
-    <row r="19" spans="1:93">
+    <row r="19" spans="1:92">
       <c r="A19">
         <v>0</v>
       </c>
@@ -5923,7 +5899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:93">
+    <row r="20" spans="1:92">
       <c r="A20">
         <v>0</v>
       </c>
@@ -6198,7 +6174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:93">
+    <row r="21" spans="1:92">
       <c r="A21">
         <v>0</v>
       </c>
@@ -6473,7 +6449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:93">
+    <row r="22" spans="1:92">
       <c r="A22">
         <v>0</v>
       </c>
@@ -6748,7 +6724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:93">
+    <row r="23" spans="1:92">
       <c r="A23">
         <v>0</v>
       </c>
@@ -7023,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:93">
+    <row r="24" spans="1:92">
       <c r="A24">
         <v>0</v>
       </c>
@@ -7300,11 +7276,8 @@
       <c r="CN24">
         <v>0</v>
       </c>
-      <c r="CO24">
-        <v>104.5546875</v>
-      </c>
     </row>
-    <row r="25" spans="1:93">
+    <row r="25" spans="1:92">
       <c r="A25">
         <v>0</v>
       </c>
@@ -7579,7 +7552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:93">
+    <row r="26" spans="1:92">
       <c r="A26">
         <v>0</v>
       </c>
@@ -7854,7 +7827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:93">
+    <row r="27" spans="1:92">
       <c r="A27">
         <v>0</v>
       </c>
@@ -8131,11 +8104,8 @@
       <c r="CN27">
         <v>1</v>
       </c>
-      <c r="CO27">
-        <v>119.734375</v>
-      </c>
     </row>
-    <row r="28" spans="1:93">
+    <row r="28" spans="1:92">
       <c r="A28">
         <v>0</v>
       </c>
@@ -8410,7 +8380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:93">
+    <row r="29" spans="1:92">
       <c r="A29">
         <v>0</v>
       </c>
@@ -8685,7 +8655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:93">
+    <row r="30" spans="1:92">
       <c r="A30">
         <v>0</v>
       </c>
@@ -8960,7 +8930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:93">
+    <row r="31" spans="1:92">
       <c r="A31">
         <v>0</v>
       </c>
@@ -9235,7 +9205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:93">
+    <row r="32" spans="1:92">
       <c r="A32">
         <v>0</v>
       </c>
@@ -9510,7 +9480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:93">
+    <row r="33" spans="1:92">
       <c r="A33">
         <v>0</v>
       </c>
@@ -9785,7 +9755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:93">
+    <row r="34" spans="1:92">
       <c r="A34">
         <v>0</v>
       </c>
@@ -10060,7 +10030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:93">
+    <row r="35" spans="1:92">
       <c r="A35">
         <v>0</v>
       </c>
@@ -10335,7 +10305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:93">
+    <row r="36" spans="1:92">
       <c r="A36">
         <v>0</v>
       </c>
@@ -10610,7 +10580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:93">
+    <row r="37" spans="1:92">
       <c r="A37">
         <v>0</v>
       </c>
@@ -10885,7 +10855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:93">
+    <row r="38" spans="1:92">
       <c r="A38">
         <v>0</v>
       </c>
@@ -11160,7 +11130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:93">
+    <row r="39" spans="1:92">
       <c r="A39">
         <v>0</v>
       </c>
@@ -11435,7 +11405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:93">
+    <row r="40" spans="1:92">
       <c r="A40">
         <v>0</v>
       </c>
@@ -11710,7 +11680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:93">
+    <row r="41" spans="1:92">
       <c r="A41">
         <v>0</v>
       </c>
@@ -11985,7 +11955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:93">
+    <row r="42" spans="1:92">
       <c r="A42">
         <v>0</v>
       </c>
@@ -12260,7 +12230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:93">
+    <row r="43" spans="1:92">
       <c r="A43">
         <v>0</v>
       </c>
@@ -12537,11 +12507,8 @@
       <c r="CN43">
         <v>1</v>
       </c>
-      <c r="CO43">
-        <v>109.4453125</v>
-      </c>
     </row>
-    <row r="44" spans="1:93">
+    <row r="44" spans="1:92">
       <c r="A44">
         <v>0</v>
       </c>
@@ -12818,11 +12785,8 @@
       <c r="CN44">
         <v>1</v>
       </c>
-      <c r="CO44">
-        <v>113.6796875</v>
-      </c>
     </row>
-    <row r="45" spans="1:93">
+    <row r="45" spans="1:92">
       <c r="A45">
         <v>0</v>
       </c>
@@ -13097,7 +13061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:93">
+    <row r="46" spans="1:92">
       <c r="A46">
         <v>0</v>
       </c>
@@ -13372,7 +13336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:93">
+    <row r="47" spans="1:92">
       <c r="A47">
         <v>0</v>
       </c>
@@ -13647,7 +13611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:93">
+    <row r="48" spans="1:92">
       <c r="A48">
         <v>0</v>
       </c>
@@ -13922,7 +13886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:93">
+    <row r="49" spans="1:92">
       <c r="A49">
         <v>0</v>
       </c>
@@ -14197,7 +14161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:93">
+    <row r="50" spans="1:92">
       <c r="A50">
         <v>0</v>
       </c>
@@ -14474,11 +14438,8 @@
       <c r="CN50">
         <v>0</v>
       </c>
-      <c r="CO50">
-        <v>119.0703125</v>
-      </c>
     </row>
-    <row r="51" spans="1:93">
+    <row r="51" spans="1:92">
       <c r="A51">
         <v>0</v>
       </c>
@@ -14753,7 +14714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:93">
+    <row r="52" spans="1:92">
       <c r="A52">
         <v>0</v>
       </c>
@@ -15028,7 +14989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:93">
+    <row r="53" spans="1:92">
       <c r="A53">
         <v>0</v>
       </c>
@@ -15303,7 +15264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:93">
+    <row r="54" spans="1:92">
       <c r="A54">
         <v>0</v>
       </c>
@@ -15580,11 +15541,8 @@
       <c r="CN54">
         <v>1</v>
       </c>
-      <c r="CO54">
-        <v>114.4765625</v>
-      </c>
     </row>
-    <row r="55" spans="1:93">
+    <row r="55" spans="1:92">
       <c r="A55">
         <v>0</v>
       </c>
@@ -15859,7 +15817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:93">
+    <row r="56" spans="1:92">
       <c r="A56">
         <v>0</v>
       </c>
@@ -16134,7 +16092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:93">
+    <row r="57" spans="1:92">
       <c r="A57">
         <v>0</v>
       </c>
@@ -16409,7 +16367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:93">
+    <row r="58" spans="1:92">
       <c r="A58">
         <v>0</v>
       </c>
@@ -16684,7 +16642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:93">
+    <row r="59" spans="1:92">
       <c r="A59">
         <v>0</v>
       </c>
@@ -16959,7 +16917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:93">
+    <row r="60" spans="1:92">
       <c r="A60">
         <v>0</v>
       </c>
@@ -17234,7 +17192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:93">
+    <row r="61" spans="1:92">
       <c r="A61">
         <v>0</v>
       </c>
@@ -17511,11 +17469,8 @@
       <c r="CN61">
         <v>1</v>
       </c>
-      <c r="CO61">
-        <v>113.8046875</v>
-      </c>
     </row>
-    <row r="62" spans="1:93">
+    <row r="62" spans="1:92">
       <c r="A62">
         <v>0</v>
       </c>
@@ -17790,7 +17745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:93">
+    <row r="63" spans="1:92">
       <c r="A63">
         <v>0</v>
       </c>
@@ -18065,7 +18020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:93">
+    <row r="64" spans="1:92">
       <c r="A64">
         <v>0</v>
       </c>
@@ -18340,7 +18295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:93">
+    <row r="65" spans="1:92">
       <c r="A65">
         <v>1</v>
       </c>
@@ -18617,11 +18572,8 @@
       <c r="CN65">
         <v>1</v>
       </c>
-      <c r="CO65">
-        <v>131.359375</v>
-      </c>
     </row>
-    <row r="66" spans="1:93">
+    <row r="66" spans="1:92">
       <c r="A66">
         <v>0</v>
       </c>
@@ -18896,7 +18848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:93">
+    <row r="67" spans="1:92">
       <c r="A67">
         <v>0</v>
       </c>
@@ -19171,7 +19123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:93">
+    <row r="68" spans="1:92">
       <c r="A68">
         <v>0</v>
       </c>
@@ -19448,11 +19400,8 @@
       <c r="CN68">
         <v>0</v>
       </c>
-      <c r="CO68">
-        <v>127.4921875</v>
-      </c>
     </row>
-    <row r="69" spans="1:93">
+    <row r="69" spans="1:92">
       <c r="A69">
         <v>0</v>
       </c>
@@ -19727,7 +19676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:93">
+    <row r="70" spans="1:92">
       <c r="A70">
         <v>1</v>
       </c>
@@ -20002,7 +19951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:93">
+    <row r="71" spans="1:92">
       <c r="A71">
         <v>0</v>
       </c>
@@ -20277,7 +20226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:93">
+    <row r="72" spans="1:92">
       <c r="A72">
         <v>0</v>
       </c>
@@ -20552,7 +20501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:93">
+    <row r="73" spans="1:92">
       <c r="A73">
         <v>0</v>
       </c>
@@ -20829,11 +20778,8 @@
       <c r="CN73">
         <v>1</v>
       </c>
-      <c r="CO73">
-        <v>110.1171875</v>
-      </c>
     </row>
-    <row r="74" spans="1:93">
+    <row r="74" spans="1:92">
       <c r="A74">
         <v>1</v>
       </c>
@@ -21110,11 +21056,8 @@
       <c r="CN74">
         <v>0</v>
       </c>
-      <c r="CO74">
-        <v>107.2734375</v>
-      </c>
     </row>
-    <row r="75" spans="1:93">
+    <row r="75" spans="1:92">
       <c r="A75">
         <v>0</v>
       </c>
@@ -21389,7 +21332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:93">
+    <row r="76" spans="1:92">
       <c r="A76">
         <v>0</v>
       </c>
@@ -21664,7 +21607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:93">
+    <row r="77" spans="1:92">
       <c r="A77">
         <v>0</v>
       </c>
@@ -21939,7 +21882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:93">
+    <row r="78" spans="1:92">
       <c r="A78">
         <v>0</v>
       </c>
@@ -22214,7 +22157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:93">
+    <row r="79" spans="1:92">
       <c r="A79">
         <v>0</v>
       </c>
@@ -22491,11 +22434,8 @@
       <c r="CN79">
         <v>0</v>
       </c>
-      <c r="CO79">
-        <v>113.0859375</v>
-      </c>
     </row>
-    <row r="80" spans="1:93">
+    <row r="80" spans="1:92">
       <c r="A80">
         <v>0</v>
       </c>
@@ -22770,7 +22710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:93">
+    <row r="81" spans="1:92">
       <c r="A81">
         <v>0</v>
       </c>
@@ -23045,7 +22985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:93">
+    <row r="82" spans="1:92">
       <c r="A82">
         <v>0</v>
       </c>
@@ -23320,7 +23260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:93">
+    <row r="83" spans="1:92">
       <c r="A83">
         <v>0</v>
       </c>
@@ -23597,11 +23537,8 @@
       <c r="CN83">
         <v>1</v>
       </c>
-      <c r="CO83">
-        <v>131.8046875</v>
-      </c>
     </row>
-    <row r="84" spans="1:93">
+    <row r="84" spans="1:92">
       <c r="A84">
         <v>1</v>
       </c>
@@ -23876,7 +23813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:93">
+    <row r="85" spans="1:92">
       <c r="A85">
         <v>0</v>
       </c>
@@ -24151,7 +24088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:93">
+    <row r="86" spans="1:92">
       <c r="A86">
         <v>0</v>
       </c>
@@ -24426,7 +24363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:93">
+    <row r="87" spans="1:92">
       <c r="A87">
         <v>0</v>
       </c>
@@ -24701,7 +24638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:93">
+    <row r="88" spans="1:92">
       <c r="A88">
         <v>0</v>
       </c>
@@ -24976,7 +24913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:93">
+    <row r="89" spans="1:92">
       <c r="A89">
         <v>0</v>
       </c>
@@ -25251,7 +25188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:93">
+    <row r="90" spans="1:92">
       <c r="A90">
         <v>0</v>
       </c>
@@ -25526,7 +25463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:93">
+    <row r="91" spans="1:92">
       <c r="A91">
         <v>0</v>
       </c>
@@ -25801,7 +25738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:93">
+    <row r="92" spans="1:92">
       <c r="A92">
         <v>0</v>
       </c>
@@ -26076,7 +26013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:93">
+    <row r="93" spans="1:92">
       <c r="A93">
         <v>0</v>
       </c>
@@ -26351,7 +26288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:93">
+    <row r="94" spans="1:92">
       <c r="A94">
         <v>0</v>
       </c>
@@ -26628,11 +26565,8 @@
       <c r="CN94">
         <v>0</v>
       </c>
-      <c r="CO94">
-        <v>116.1796875</v>
-      </c>
     </row>
-    <row r="95" spans="1:93">
+    <row r="95" spans="1:92">
       <c r="A95">
         <v>0</v>
       </c>
@@ -26907,7 +26841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:93">
+    <row r="96" spans="1:92">
       <c r="A96">
         <v>0</v>
       </c>
@@ -27184,11 +27118,8 @@
       <c r="CN96">
         <v>1</v>
       </c>
-      <c r="CO96">
-        <v>115.859375</v>
-      </c>
     </row>
-    <row r="97" spans="1:93">
+    <row r="97" spans="1:92">
       <c r="A97">
         <v>0</v>
       </c>
@@ -27463,7 +27394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:93">
+    <row r="98" spans="1:92">
       <c r="A98">
         <v>0</v>
       </c>
@@ -27738,7 +27669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:93">
+    <row r="99" spans="1:92">
       <c r="A99">
         <v>0</v>
       </c>
@@ -28013,7 +27944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:93">
+    <row r="100" spans="1:92">
       <c r="A100">
         <v>0</v>
       </c>
@@ -28288,7 +28219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:93">
+    <row r="101" spans="1:92">
       <c r="A101">
         <v>0</v>
       </c>
@@ -28563,7 +28494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:93">
+    <row r="102" spans="1:92">
       <c r="A102">
         <v>0</v>
       </c>
@@ -28838,7 +28769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:93">
+    <row r="103" spans="1:92">
       <c r="A103">
         <v>0</v>
       </c>
@@ -29113,7 +29044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:93">
+    <row r="104" spans="1:92">
       <c r="A104">
         <v>0</v>
       </c>
@@ -29388,7 +29319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:93">
+    <row r="105" spans="1:92">
       <c r="A105">
         <v>0</v>
       </c>
@@ -29663,7 +29594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:93">
+    <row r="106" spans="1:92">
       <c r="A106">
         <v>0</v>
       </c>
@@ -29938,7 +29869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:93">
+    <row r="107" spans="1:92">
       <c r="A107">
         <v>0</v>
       </c>
@@ -30215,11 +30146,8 @@
       <c r="CN107">
         <v>1</v>
       </c>
-      <c r="CO107">
-        <v>119.5078125</v>
-      </c>
     </row>
-    <row r="108" spans="1:93">
+    <row r="108" spans="1:92">
       <c r="A108">
         <v>0</v>
       </c>
@@ -30494,7 +30422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:93">
+    <row r="109" spans="1:92">
       <c r="A109">
         <v>0</v>
       </c>
@@ -30771,11 +30699,8 @@
       <c r="CN109">
         <v>0</v>
       </c>
-      <c r="CO109">
-        <v>101.6796875</v>
-      </c>
     </row>
-    <row r="110" spans="1:93">
+    <row r="110" spans="1:92">
       <c r="A110">
         <v>0</v>
       </c>
@@ -31050,7 +30975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:93">
+    <row r="111" spans="1:92">
       <c r="A111">
         <v>0</v>
       </c>
@@ -31325,7 +31250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:93">
+    <row r="112" spans="1:92">
       <c r="A112">
         <v>0</v>
       </c>
@@ -31602,11 +31527,8 @@
       <c r="CN112">
         <v>0</v>
       </c>
-      <c r="CO112">
-        <v>110.9921875</v>
-      </c>
     </row>
-    <row r="113" spans="1:93">
+    <row r="113" spans="1:92">
       <c r="A113">
         <v>0</v>
       </c>
@@ -31881,7 +31803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:93">
+    <row r="114" spans="1:92">
       <c r="A114">
         <v>0</v>
       </c>
@@ -32158,11 +32080,8 @@
       <c r="CN114">
         <v>0</v>
       </c>
-      <c r="CO114">
-        <v>107.921875</v>
-      </c>
     </row>
-    <row r="115" spans="1:93">
+    <row r="115" spans="1:92">
       <c r="A115">
         <v>0</v>
       </c>
@@ -32437,7 +32356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:93">
+    <row r="116" spans="1:92">
       <c r="A116">
         <v>0</v>
       </c>
@@ -32712,7 +32631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:93">
+    <row r="117" spans="1:92">
       <c r="A117">
         <v>0</v>
       </c>
@@ -32989,11 +32908,8 @@
       <c r="CN117">
         <v>1</v>
       </c>
-      <c r="CO117">
-        <v>109.3046875</v>
-      </c>
     </row>
-    <row r="118" spans="1:93">
+    <row r="118" spans="1:92">
       <c r="A118">
         <v>0</v>
       </c>
@@ -33268,7 +33184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:93">
+    <row r="119" spans="1:92">
       <c r="A119">
         <v>0</v>
       </c>
@@ -33543,7 +33459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:93">
+    <row r="120" spans="1:92">
       <c r="A120">
         <v>0</v>
       </c>
@@ -33818,7 +33734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:93">
+    <row r="121" spans="1:92">
       <c r="A121">
         <v>0</v>
       </c>
@@ -34093,7 +34009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:93">
+    <row r="122" spans="1:92">
       <c r="A122">
         <v>0</v>
       </c>
@@ -34368,7 +34284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:93">
+    <row r="123" spans="1:92">
       <c r="A123">
         <v>0</v>
       </c>
@@ -34643,7 +34559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:93">
+    <row r="124" spans="1:92">
       <c r="A124">
         <v>0</v>
       </c>
@@ -34918,7 +34834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:93">
+    <row r="125" spans="1:92">
       <c r="A125">
         <v>0</v>
       </c>
@@ -35193,7 +35109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:93">
+    <row r="126" spans="1:92">
       <c r="A126">
         <v>0</v>
       </c>
@@ -35468,7 +35384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:93">
+    <row r="127" spans="1:92">
       <c r="A127">
         <v>0</v>
       </c>
@@ -35743,804 +35659,504 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:93">
+    <row r="128" spans="1:92">
       <c r="CN128">
         <v>1</v>
       </c>
-      <c r="CO128">
-        <v>120.4921875</v>
-      </c>
     </row>
-    <row r="129" spans="92:93">
+    <row r="129" spans="92:92">
       <c r="CN129">
         <v>1</v>
       </c>
-      <c r="CO129">
-        <v>107.5546875</v>
-      </c>
     </row>
-    <row r="130" spans="92:93">
+    <row r="130" spans="92:92">
       <c r="CN130">
         <v>1</v>
       </c>
-      <c r="CO130">
-        <v>107.0703125</v>
-      </c>
     </row>
-    <row r="131" spans="92:93">
+    <row r="131" spans="92:92">
       <c r="CN131">
         <v>1</v>
       </c>
-      <c r="CO131">
-        <v>129.3671875</v>
-      </c>
     </row>
-    <row r="132" spans="92:93">
+    <row r="132" spans="92:92">
       <c r="CN132">
         <v>1</v>
       </c>
-      <c r="CO132">
-        <v>125.015625</v>
-      </c>
     </row>
-    <row r="133" spans="92:93">
+    <row r="133" spans="92:92">
       <c r="CN133">
         <v>1</v>
       </c>
-      <c r="CO133">
-        <v>117.8203125</v>
-      </c>
     </row>
-    <row r="134" spans="92:93">
+    <row r="134" spans="92:92">
       <c r="CN134">
         <v>0</v>
       </c>
-      <c r="CO134">
-        <v>118.53125</v>
-      </c>
     </row>
-    <row r="135" spans="92:93">
+    <row r="135" spans="92:92">
       <c r="CN135">
         <v>1</v>
       </c>
-      <c r="CO135">
-        <v>129.3046875</v>
-      </c>
     </row>
-    <row r="136" spans="92:93">
+    <row r="136" spans="92:92">
       <c r="CN136">
         <v>1</v>
       </c>
-      <c r="CO136">
-        <v>119.3046875</v>
-      </c>
     </row>
-    <row r="137" spans="92:93">
+    <row r="137" spans="92:92">
       <c r="CN137">
         <v>0</v>
       </c>
-      <c r="CO137">
-        <v>106.3203125</v>
-      </c>
     </row>
-    <row r="138" spans="92:93">
+    <row r="138" spans="92:92">
       <c r="CN138">
         <v>0</v>
       </c>
-      <c r="CO138">
-        <v>118.5703125</v>
-      </c>
     </row>
-    <row r="139" spans="92:93">
+    <row r="139" spans="92:92">
       <c r="CN139">
         <v>0</v>
       </c>
-      <c r="CO139">
-        <v>109.609375</v>
-      </c>
     </row>
-    <row r="140" spans="92:93">
+    <row r="140" spans="92:92">
       <c r="CN140">
         <v>0</v>
       </c>
-      <c r="CO140">
-        <v>109.34375</v>
-      </c>
     </row>
-    <row r="141" spans="92:93">
+    <row r="141" spans="92:92">
       <c r="CN141">
         <v>1</v>
       </c>
-      <c r="CO141">
-        <v>126.8671875</v>
-      </c>
     </row>
-    <row r="142" spans="92:93">
+    <row r="142" spans="92:92">
       <c r="CN142">
         <v>1</v>
       </c>
-      <c r="CO142">
-        <v>110.4453125</v>
-      </c>
     </row>
-    <row r="143" spans="92:93">
+    <row r="143" spans="92:92">
       <c r="CN143">
         <v>0</v>
       </c>
-      <c r="CO143">
-        <v>118.1796875</v>
-      </c>
     </row>
-    <row r="144" spans="92:93">
+    <row r="144" spans="92:92">
       <c r="CN144">
         <v>1</v>
       </c>
-      <c r="CO144">
-        <v>123.5546875</v>
-      </c>
     </row>
-    <row r="145" spans="92:93">
+    <row r="145" spans="92:92">
       <c r="CN145">
         <v>1</v>
       </c>
-      <c r="CO145">
-        <v>117.8046875</v>
-      </c>
     </row>
-    <row r="146" spans="92:93">
+    <row r="146" spans="92:92">
       <c r="CN146">
         <v>0</v>
       </c>
-      <c r="CO146">
-        <v>109.6015625</v>
-      </c>
     </row>
-    <row r="147" spans="92:93">
+    <row r="147" spans="92:92">
       <c r="CN147">
         <v>0</v>
       </c>
-      <c r="CO147">
-        <v>119.1171875</v>
-      </c>
     </row>
-    <row r="148" spans="92:93">
+    <row r="148" spans="92:92">
       <c r="CN148">
         <v>1</v>
       </c>
-      <c r="CO148">
-        <v>129.0546875</v>
-      </c>
     </row>
-    <row r="149" spans="92:93">
+    <row r="149" spans="92:92">
       <c r="CN149">
         <v>1</v>
       </c>
-      <c r="CO149">
-        <v>117.0390625</v>
-      </c>
     </row>
-    <row r="150" spans="92:93">
+    <row r="150" spans="92:92">
       <c r="CN150">
         <v>0</v>
       </c>
-      <c r="CO150">
-        <v>97.9296875</v>
-      </c>
     </row>
-    <row r="151" spans="92:93">
+    <row r="151" spans="92:92">
       <c r="CN151">
         <v>0</v>
       </c>
-      <c r="CO151">
-        <v>117.53125</v>
-      </c>
     </row>
-    <row r="152" spans="92:93">
+    <row r="152" spans="92:92">
       <c r="CN152">
         <v>0</v>
       </c>
-      <c r="CO152">
-        <v>112.265625</v>
-      </c>
     </row>
-    <row r="153" spans="92:93">
+    <row r="153" spans="92:92">
       <c r="CN153">
         <v>0</v>
       </c>
-      <c r="CO153">
-        <v>112.0390625</v>
-      </c>
     </row>
-    <row r="154" spans="92:93">
+    <row r="154" spans="92:92">
       <c r="CN154">
         <v>1</v>
       </c>
-      <c r="CO154">
-        <v>122.828125</v>
-      </c>
     </row>
-    <row r="155" spans="92:93">
+    <row r="155" spans="92:92">
       <c r="CN155">
         <v>0</v>
       </c>
-      <c r="CO155">
-        <v>123.859375</v>
-      </c>
     </row>
-    <row r="156" spans="92:93">
+    <row r="156" spans="92:92">
       <c r="CN156">
         <v>1</v>
       </c>
-      <c r="CO156">
-        <v>120.4609375</v>
-      </c>
     </row>
-    <row r="157" spans="92:93">
+    <row r="157" spans="92:92">
       <c r="CN157">
         <v>1</v>
       </c>
-      <c r="CO157">
-        <v>118.0546875</v>
-      </c>
     </row>
-    <row r="158" spans="92:93">
+    <row r="158" spans="92:92">
       <c r="CN158">
         <v>1</v>
       </c>
-      <c r="CO158">
-        <v>122.0546875</v>
-      </c>
     </row>
-    <row r="159" spans="92:93">
+    <row r="159" spans="92:92">
       <c r="CN159">
         <v>1</v>
       </c>
-      <c r="CO159">
-        <v>122.0546875</v>
-      </c>
     </row>
-    <row r="160" spans="92:93">
+    <row r="160" spans="92:92">
       <c r="CN160">
         <v>1</v>
       </c>
-      <c r="CO160">
-        <v>118.5546875</v>
-      </c>
     </row>
-    <row r="161" spans="92:93">
+    <row r="161" spans="92:92">
       <c r="CN161">
         <v>0</v>
       </c>
-      <c r="CO161">
-        <v>116.4375</v>
-      </c>
     </row>
-    <row r="162" spans="92:93">
+    <row r="162" spans="92:92">
       <c r="CN162">
         <v>0</v>
       </c>
-      <c r="CO162">
-        <v>109.2109375</v>
-      </c>
     </row>
-    <row r="163" spans="92:93">
+    <row r="163" spans="92:92">
       <c r="CN163">
         <v>1</v>
       </c>
-      <c r="CO163">
-        <v>116.5546875</v>
-      </c>
     </row>
-    <row r="164" spans="92:93">
+    <row r="164" spans="92:92">
       <c r="CN164">
         <v>1</v>
       </c>
-      <c r="CO164">
-        <v>121.7421875</v>
-      </c>
     </row>
-    <row r="165" spans="92:93">
+    <row r="165" spans="92:92">
       <c r="CN165">
         <v>1</v>
       </c>
-      <c r="CO165">
-        <v>130.8046875</v>
-      </c>
     </row>
-    <row r="166" spans="92:93">
+    <row r="166" spans="92:92">
       <c r="CN166">
         <v>0</v>
       </c>
-      <c r="CO166">
-        <v>108.265625</v>
-      </c>
     </row>
-    <row r="167" spans="92:93">
+    <row r="167" spans="92:92">
       <c r="CN167">
         <v>1</v>
       </c>
-      <c r="CO167">
-        <v>119.5703125</v>
-      </c>
     </row>
-    <row r="168" spans="92:93">
+    <row r="168" spans="92:92">
       <c r="CN168">
         <v>0</v>
       </c>
-      <c r="CO168">
-        <v>115.4921875</v>
-      </c>
     </row>
-    <row r="169" spans="92:93">
+    <row r="169" spans="92:92">
       <c r="CN169">
         <v>1</v>
       </c>
-      <c r="CO169">
-        <v>122.1953125</v>
-      </c>
     </row>
-    <row r="170" spans="92:93">
+    <row r="170" spans="92:92">
       <c r="CN170">
         <v>1</v>
       </c>
-      <c r="CO170">
-        <v>125.4296875</v>
-      </c>
     </row>
-    <row r="171" spans="92:93">
+    <row r="171" spans="92:92">
       <c r="CN171">
         <v>0</v>
       </c>
-      <c r="CO171">
-        <v>108.3046875</v>
-      </c>
     </row>
-    <row r="172" spans="92:93">
+    <row r="172" spans="92:92">
       <c r="CN172">
         <v>0</v>
       </c>
-      <c r="CO172">
-        <v>112.9375</v>
-      </c>
     </row>
-    <row r="173" spans="92:93">
+    <row r="173" spans="92:92">
       <c r="CN173">
         <v>1</v>
       </c>
-      <c r="CO173">
-        <v>105.8046875</v>
-      </c>
     </row>
-    <row r="174" spans="92:93">
+    <row r="174" spans="92:92">
       <c r="CN174">
         <v>1</v>
       </c>
-      <c r="CO174">
-        <v>118.0546875</v>
-      </c>
     </row>
-    <row r="175" spans="92:93">
+    <row r="175" spans="92:92">
       <c r="CN175">
         <v>1</v>
       </c>
-      <c r="CO175">
-        <v>130.6796875</v>
-      </c>
     </row>
-    <row r="176" spans="92:93">
+    <row r="176" spans="92:92">
       <c r="CN176">
         <v>1</v>
       </c>
-      <c r="CO176">
-        <v>122.5546875</v>
-      </c>
     </row>
-    <row r="177" spans="92:93">
+    <row r="177" spans="92:92">
       <c r="CN177">
         <v>1</v>
       </c>
-      <c r="CO177">
-        <v>130.0859375</v>
-      </c>
     </row>
-    <row r="178" spans="92:93">
+    <row r="178" spans="92:92">
       <c r="CN178">
         <v>0</v>
       </c>
-      <c r="CO178">
-        <v>117.3046875</v>
-      </c>
     </row>
-    <row r="179" spans="92:93">
+    <row r="179" spans="92:92">
       <c r="CN179">
         <v>0</v>
       </c>
-      <c r="CO179">
-        <v>122.2421875</v>
-      </c>
     </row>
-    <row r="180" spans="92:93">
+    <row r="180" spans="92:92">
       <c r="CN180">
         <v>1</v>
       </c>
-      <c r="CO180">
-        <v>113.4296875</v>
-      </c>
     </row>
-    <row r="181" spans="92:93">
+    <row r="181" spans="92:92">
       <c r="CN181">
         <v>1</v>
       </c>
-      <c r="CO181">
-        <v>129.8125</v>
-      </c>
     </row>
-    <row r="182" spans="92:93">
+    <row r="182" spans="92:92">
       <c r="CN182">
         <v>0</v>
       </c>
-      <c r="CO182">
-        <v>114.8046875</v>
-      </c>
     </row>
-    <row r="183" spans="92:93">
+    <row r="183" spans="92:92">
       <c r="CN183">
         <v>0</v>
       </c>
-      <c r="CO183">
-        <v>121.8046875</v>
-      </c>
     </row>
-    <row r="184" spans="92:93">
+    <row r="184" spans="92:92">
       <c r="CN184">
         <v>0</v>
       </c>
-      <c r="CO184">
-        <v>109.8046875</v>
-      </c>
     </row>
-    <row r="185" spans="92:93">
+    <row r="185" spans="92:92">
       <c r="CN185">
         <v>1</v>
       </c>
-      <c r="CO185">
-        <v>121.7421875</v>
-      </c>
     </row>
-    <row r="186" spans="92:93">
+    <row r="186" spans="92:92">
       <c r="CN186">
         <v>1</v>
       </c>
-      <c r="CO186">
-        <v>119.0703125</v>
-      </c>
     </row>
-    <row r="187" spans="92:93">
+    <row r="187" spans="92:92">
       <c r="CN187">
         <v>1</v>
       </c>
-      <c r="CO187">
-        <v>117.6953125</v>
-      </c>
     </row>
-    <row r="188" spans="92:93">
+    <row r="188" spans="92:92">
       <c r="CN188">
         <v>0</v>
       </c>
-      <c r="CO188">
-        <v>113.1796875</v>
-      </c>
     </row>
-    <row r="189" spans="92:93">
+    <row r="189" spans="92:92">
       <c r="CN189">
         <v>1</v>
       </c>
-      <c r="CO189">
-        <v>120.3828125</v>
-      </c>
     </row>
-    <row r="190" spans="92:93">
+    <row r="190" spans="92:92">
       <c r="CN190">
         <v>0</v>
       </c>
-      <c r="CO190">
-        <v>114.4296875</v>
-      </c>
     </row>
-    <row r="191" spans="92:93">
+    <row r="191" spans="92:92">
       <c r="CN191">
         <v>1</v>
       </c>
-      <c r="CO191">
-        <v>119.0546875</v>
-      </c>
     </row>
-    <row r="192" spans="92:93">
+    <row r="192" spans="92:92">
       <c r="CN192">
         <v>1</v>
       </c>
-      <c r="CO192">
-        <v>105.5546875</v>
-      </c>
     </row>
-    <row r="193" spans="92:93">
+    <row r="193" spans="92:92">
       <c r="CN193">
         <v>1</v>
       </c>
-      <c r="CO193">
-        <v>114.3046875</v>
-      </c>
     </row>
-    <row r="194" spans="92:93">
+    <row r="194" spans="92:92">
       <c r="CN194">
         <v>1</v>
       </c>
-      <c r="CO194">
-        <v>117.3046875</v>
-      </c>
     </row>
-    <row r="195" spans="92:93">
+    <row r="195" spans="92:92">
       <c r="CN195">
         <v>1</v>
       </c>
-      <c r="CO195">
-        <v>-1678297235044766</v>
-      </c>
     </row>
-    <row r="196" spans="92:93">
+    <row r="196" spans="92:92">
       <c r="CN196">
         <v>1</v>
       </c>
-      <c r="CO196">
-        <v>119.1875</v>
-      </c>
     </row>
-    <row r="197" spans="92:93">
+    <row r="197" spans="92:92">
       <c r="CN197">
         <v>1</v>
       </c>
-      <c r="CO197">
-        <v>117.8828125</v>
-      </c>
     </row>
-    <row r="198" spans="92:93">
+    <row r="198" spans="92:92">
       <c r="CN198">
         <v>0</v>
       </c>
-      <c r="CO198">
-        <v>111.875</v>
-      </c>
     </row>
-    <row r="199" spans="92:93">
+    <row r="199" spans="92:92">
       <c r="CN199">
         <v>1</v>
       </c>
-      <c r="CO199">
-        <v>113.0546875</v>
-      </c>
     </row>
-    <row r="200" spans="92:93">
+    <row r="200" spans="92:92">
       <c r="CN200">
         <v>1</v>
       </c>
-      <c r="CO200">
-        <v>130.7578125</v>
-      </c>
     </row>
-    <row r="201" spans="92:93">
+    <row r="201" spans="92:92">
       <c r="CN201">
         <v>1</v>
       </c>
-      <c r="CO201">
-        <v>117.5546875</v>
-      </c>
     </row>
-    <row r="202" spans="92:93">
+    <row r="202" spans="92:92">
       <c r="CN202">
         <v>1</v>
       </c>
-      <c r="CO202">
-        <v>123.6953125</v>
-      </c>
     </row>
-    <row r="203" spans="92:93">
+    <row r="203" spans="92:92">
       <c r="CN203">
         <v>1</v>
       </c>
-      <c r="CO203">
-        <v>120.0546875</v>
-      </c>
     </row>
-    <row r="204" spans="92:93">
+    <row r="204" spans="92:92">
       <c r="CN204">
         <v>1</v>
       </c>
-      <c r="CO204">
-        <v>116.0546875</v>
-      </c>
     </row>
-    <row r="205" spans="92:93">
+    <row r="205" spans="92:92">
       <c r="CN205">
         <v>1</v>
       </c>
-      <c r="CO205">
-        <v>115.4921875</v>
-      </c>
     </row>
-    <row r="206" spans="92:93">
+    <row r="206" spans="92:92">
       <c r="CN206">
         <v>1</v>
       </c>
-      <c r="CO206">
-        <v>112.3046875</v>
-      </c>
     </row>
-    <row r="207" spans="92:93">
+    <row r="207" spans="92:92">
       <c r="CN207">
         <v>1</v>
       </c>
-      <c r="CO207">
-        <v>114.6015625</v>
-      </c>
     </row>
-    <row r="208" spans="92:93">
+    <row r="208" spans="92:92">
       <c r="CN208">
         <v>0</v>
       </c>
-      <c r="CO208">
-        <v>107.9296875</v>
-      </c>
     </row>
-    <row r="209" spans="92:93">
+    <row r="209" spans="92:92">
       <c r="CN209">
         <v>0</v>
       </c>
-      <c r="CO209">
-        <v>113.7109375</v>
-      </c>
     </row>
-    <row r="210" spans="92:93">
+    <row r="210" spans="92:92">
       <c r="CN210">
         <v>1</v>
       </c>
-      <c r="CO210">
-        <v>117.4375</v>
-      </c>
     </row>
-    <row r="211" spans="92:93">
+    <row r="211" spans="92:92">
       <c r="CN211">
         <v>1</v>
       </c>
-      <c r="CO211">
-        <v>110.5234375</v>
-      </c>
     </row>
-    <row r="212" spans="92:93">
+    <row r="212" spans="92:92">
       <c r="CN212">
         <v>1</v>
       </c>
-      <c r="CO212">
-        <v>115.5546875</v>
-      </c>
     </row>
-    <row r="213" spans="92:93">
+    <row r="213" spans="92:92">
       <c r="CN213">
         <v>1</v>
       </c>
-      <c r="CO213">
-        <v>120.8671875</v>
-      </c>
     </row>
-    <row r="214" spans="92:93">
+    <row r="214" spans="92:92">
       <c r="CN214">
         <v>1</v>
       </c>
-      <c r="CO214">
-        <v>127.3984375</v>
-      </c>
     </row>
-    <row r="215" spans="92:93">
+    <row r="215" spans="92:92">
       <c r="CN215">
         <v>1</v>
       </c>
-      <c r="CO215">
-        <v>123.0546875</v>
-      </c>
     </row>
-    <row r="216" spans="92:93">
+    <row r="216" spans="92:92">
       <c r="CN216">
         <v>0</v>
       </c>
-      <c r="CO216">
-        <v>112.7421875</v>
-      </c>
     </row>
-    <row r="217" spans="92:93">
+    <row r="217" spans="92:92">
       <c r="CN217">
         <v>0</v>
       </c>
-      <c r="CO217">
-        <v>106.5546875</v>
-      </c>
     </row>
-    <row r="218" spans="92:93">
+    <row r="218" spans="92:92">
       <c r="CN218">
         <v>1</v>
       </c>
-      <c r="CO218">
-        <v>441342299198490.1</v>
-      </c>
     </row>
-    <row r="219" spans="92:93">
+    <row r="219" spans="92:92">
       <c r="CN219">
         <v>1</v>
       </c>
-      <c r="CO219">
-        <v>106.8515625</v>
-      </c>
     </row>
-    <row r="220" spans="92:93">
+    <row r="220" spans="92:92">
       <c r="CN220">
         <v>0</v>
       </c>
-      <c r="CO220">
-        <v>109.8671875</v>
-      </c>
     </row>
-    <row r="221" spans="92:93">
+    <row r="221" spans="92:92">
       <c r="CN221">
         <v>1</v>
       </c>
-      <c r="CO221">
-        <v>113.1796875</v>
-      </c>
     </row>
-    <row r="222" spans="92:93">
+    <row r="222" spans="92:92">
       <c r="CN222">
         <v>0</v>
       </c>
-      <c r="CO222">
-        <v>114.5546875</v>
-      </c>
     </row>
-    <row r="223" spans="92:93">
+    <row r="223" spans="92:92">
       <c r="CN223">
         <v>1</v>
       </c>
-      <c r="CO223">
-        <v>112.5546875</v>
-      </c>
     </row>
-    <row r="224" spans="92:93">
+    <row r="224" spans="92:92">
       <c r="CN224">
         <v>0</v>
       </c>
-      <c r="CO224">
-        <v>112.9765625</v>
-      </c>
     </row>
-    <row r="225" spans="92:93">
+    <row r="225" spans="92:92">
       <c r="CN225">
         <v>0</v>
       </c>
-      <c r="CO225">
-        <v>115.1484375</v>
-      </c>
     </row>
-    <row r="226" spans="92:93">
+    <row r="226" spans="92:92">
       <c r="CN226">
         <v>1</v>
       </c>
-      <c r="CO226">
-        <v>113.1796875</v>
-      </c>
     </row>
-    <row r="227" spans="92:93">
+    <row r="227" spans="92:92">
       <c r="CN227">
         <v>0</v>
-      </c>
-      <c r="CO227">
-        <v>108.8671875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>